<commit_message>
Merge 6001030110 and 6001030130 and 6001030140 and 6001030200.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/600.10.30.200_VerifyTheDeviceSiteIdCanBeStored.xlsx
+++ b/NformTester/NformTester/Keywordscripts/600.10.30.200_VerifyTheDeviceSiteIdCanBeStored.xlsx
@@ -1260,7 +1260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7971" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8051" uniqueCount="899">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -4011,6 +4011,14 @@
   </si>
   <si>
     <t>good2</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pause</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -4614,10 +4622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O93"/>
+  <dimension ref="A1:O114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4817,7 +4825,7 @@
         <v>803</v>
       </c>
       <c r="B7" s="4">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="C7" s="3">
         <v>6</v>
@@ -5566,7 +5574,7 @@
       <c r="M32" s="20"/>
       <c r="N32" s="16"/>
     </row>
-    <row r="33" spans="3:14">
+    <row r="33" spans="3:14" s="18" customFormat="1" ht="14.25">
       <c r="C33" s="3">
         <v>32</v>
       </c>
@@ -5577,12 +5585,12 @@
         <v>559</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>17</v>
+        <v>874</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H33" s="23"/>
+        <v>866</v>
+      </c>
+      <c r="H33" s="15"/>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
       <c r="K33" s="20"/>
@@ -5590,7 +5598,7 @@
       <c r="M33" s="20"/>
       <c r="N33" s="16"/>
     </row>
-    <row r="34" spans="3:14" s="18" customFormat="1">
+    <row r="34" spans="3:14">
       <c r="C34" s="3">
         <v>33</v>
       </c>
@@ -5598,23 +5606,21 @@
         <v>864</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>865</v>
+        <v>559</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>621</v>
+        <v>17</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H34" s="20" t="s">
-        <v>881</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H34" s="23"/>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
       <c r="M34" s="20"/>
-      <c r="N34" s="27"/>
+      <c r="N34" s="16"/>
     </row>
     <row r="35" spans="3:14" s="18" customFormat="1" ht="14.25">
       <c r="C35" s="3">
@@ -5627,7 +5633,7 @@
         <v>865</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>203</v>
+        <v>100</v>
       </c>
       <c r="G35" s="20" t="s">
         <v>866</v>
@@ -5638,25 +5644,23 @@
       <c r="K35" s="20"/>
       <c r="L35" s="20"/>
       <c r="M35" s="20"/>
-      <c r="N35" s="27"/>
+      <c r="N35" s="16"/>
     </row>
-    <row r="36" spans="3:14" s="18" customFormat="1">
+    <row r="36" spans="3:14" s="18" customFormat="1" ht="14.25">
       <c r="C36" s="3">
         <v>35</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>864</v>
+        <v>896</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>559</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>867</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>866</v>
-      </c>
-      <c r="H36" s="20"/>
+        <v>897</v>
+      </c>
+      <c r="F36" s="20">
+        <v>2</v>
+      </c>
+      <c r="G36" s="20"/>
+      <c r="H36" s="15"/>
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
       <c r="K36" s="20"/>
@@ -5669,26 +5673,20 @@
         <v>36</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>864</v>
+        <v>830</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>559</v>
+        <v>19</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>868</v>
+        <v>22</v>
       </c>
       <c r="G37" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" s="23" t="s">
-        <v>869</v>
-      </c>
-      <c r="I37" s="23" t="s">
-        <v>851</v>
-      </c>
-      <c r="J37" s="23" t="s">
-        <v>894</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H37" s="23"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
       <c r="M37" s="20"/>
@@ -5699,16 +5697,16 @@
         <v>37</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>864</v>
+        <v>830</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>559</v>
+        <v>19</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>870</v>
+        <v>79</v>
       </c>
       <c r="G38" s="20" t="s">
-        <v>871</v>
+        <v>2</v>
       </c>
       <c r="H38" s="23"/>
       <c r="I38" s="20"/>
@@ -5718,7 +5716,7 @@
       <c r="M38" s="20"/>
       <c r="N38" s="16"/>
     </row>
-    <row r="39" spans="3:14">
+    <row r="39" spans="3:14" s="18" customFormat="1">
       <c r="C39" s="3">
         <v>38</v>
       </c>
@@ -5726,29 +5724,25 @@
         <v>864</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>559</v>
+        <v>865</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>870</v>
+        <v>621</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H39" s="23" t="s">
-        <v>854</v>
-      </c>
-      <c r="I39" s="23" t="s">
-        <v>851</v>
-      </c>
-      <c r="J39" s="20" t="b">
-        <v>1</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>881</v>
+      </c>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
       <c r="K39" s="20"/>
       <c r="L39" s="20"/>
       <c r="M39" s="20"/>
-      <c r="N39" s="16"/>
+      <c r="N39" s="27"/>
     </row>
-    <row r="40" spans="3:14" s="18" customFormat="1">
+    <row r="40" spans="3:14" s="18" customFormat="1" ht="14.25">
       <c r="C40" s="3">
         <v>39</v>
       </c>
@@ -5756,48 +5750,40 @@
         <v>864</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>559</v>
+        <v>865</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>872</v>
+        <v>203</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H40" s="23" t="s">
-        <v>855</v>
-      </c>
-      <c r="I40" s="23" t="s">
-        <v>851</v>
-      </c>
-      <c r="J40" s="20" t="b">
-        <v>1</v>
-      </c>
+        <v>866</v>
+      </c>
+      <c r="H40" s="15"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
       <c r="K40" s="20"/>
       <c r="L40" s="20"/>
       <c r="M40" s="20"/>
-      <c r="N40" s="16"/>
+      <c r="N40" s="27"/>
     </row>
     <row r="41" spans="3:14" s="18" customFormat="1">
       <c r="C41" s="3">
         <v>40</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>896</v>
+        <v>864</v>
       </c>
       <c r="E41" s="23" t="s">
         <v>559</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>872</v>
-      </c>
-      <c r="G41" s="23" t="s">
-        <v>884</v>
-      </c>
-      <c r="H41" s="23" t="s">
-        <v>883</v>
-      </c>
-      <c r="I41" s="23"/>
+        <v>867</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>866</v>
+      </c>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
       <c r="J41" s="20"/>
       <c r="K41" s="20"/>
       <c r="L41" s="20"/>
@@ -5815,14 +5801,20 @@
         <v>559</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>17</v>
+        <v>868</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H42" s="23"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
+        <v>7</v>
+      </c>
+      <c r="H42" s="23" t="s">
+        <v>869</v>
+      </c>
+      <c r="I42" s="23" t="s">
+        <v>851</v>
+      </c>
+      <c r="J42" s="23" t="s">
+        <v>894</v>
+      </c>
       <c r="K42" s="20"/>
       <c r="L42" s="20"/>
       <c r="M42" s="20"/>
@@ -5836,25 +5828,23 @@
         <v>864</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>865</v>
+        <v>559</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>621</v>
+        <v>870</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H43" s="20" t="s">
-        <v>881</v>
-      </c>
+        <v>871</v>
+      </c>
+      <c r="H43" s="23"/>
       <c r="I43" s="20"/>
       <c r="J43" s="20"/>
       <c r="K43" s="20"/>
       <c r="L43" s="20"/>
       <c r="M43" s="20"/>
-      <c r="N43" s="27"/>
+      <c r="N43" s="16"/>
     </row>
-    <row r="44" spans="3:14" s="18" customFormat="1" ht="14.25">
+    <row r="44" spans="3:14">
       <c r="C44" s="3">
         <v>43</v>
       </c>
@@ -5862,21 +5852,27 @@
         <v>864</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>865</v>
+        <v>559</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>203</v>
+        <v>870</v>
       </c>
       <c r="G44" s="20" t="s">
-        <v>866</v>
-      </c>
-      <c r="H44" s="15"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
+        <v>7</v>
+      </c>
+      <c r="H44" s="23" t="s">
+        <v>854</v>
+      </c>
+      <c r="I44" s="20" t="s">
+        <v>853</v>
+      </c>
+      <c r="J44" s="20" t="b">
+        <v>1</v>
+      </c>
       <c r="K44" s="20"/>
       <c r="L44" s="20"/>
       <c r="M44" s="20"/>
-      <c r="N44" s="27"/>
+      <c r="N44" s="16"/>
     </row>
     <row r="45" spans="3:14" s="18" customFormat="1">
       <c r="C45" s="3">
@@ -5889,14 +5885,20 @@
         <v>559</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>867</v>
+        <v>872</v>
       </c>
       <c r="G45" s="20" t="s">
-        <v>866</v>
-      </c>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
+        <v>7</v>
+      </c>
+      <c r="H45" s="23" t="s">
+        <v>855</v>
+      </c>
+      <c r="I45" s="23" t="s">
+        <v>851</v>
+      </c>
+      <c r="J45" s="20" t="b">
+        <v>1</v>
+      </c>
       <c r="K45" s="20"/>
       <c r="L45" s="20"/>
       <c r="M45" s="20"/>
@@ -5913,50 +5915,38 @@
         <v>559</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>870</v>
-      </c>
-      <c r="G46" s="20" t="s">
-        <v>7</v>
+        <v>872</v>
+      </c>
+      <c r="G46" s="23" t="s">
+        <v>884</v>
       </c>
       <c r="H46" s="23" t="s">
-        <v>854</v>
-      </c>
-      <c r="I46" s="23" t="s">
-        <v>851</v>
-      </c>
-      <c r="J46" s="20" t="b">
-        <v>1</v>
-      </c>
+        <v>883</v>
+      </c>
+      <c r="I46" s="23"/>
+      <c r="J46" s="20"/>
       <c r="K46" s="20"/>
       <c r="L46" s="20"/>
       <c r="M46" s="20"/>
       <c r="N46" s="16"/>
     </row>
-    <row r="47" spans="3:14" s="18" customFormat="1">
+    <row r="47" spans="3:14" s="18" customFormat="1" ht="14.25">
       <c r="C47" s="3">
         <v>46</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>864</v>
+        <v>892</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>559</v>
-      </c>
-      <c r="F47" s="20" t="s">
-        <v>874</v>
-      </c>
-      <c r="G47" s="23" t="s">
-        <v>885</v>
-      </c>
-      <c r="H47" s="23" t="s">
-        <v>886</v>
-      </c>
-      <c r="I47" s="23" t="s">
-        <v>851</v>
-      </c>
-      <c r="J47" s="23" t="s">
-        <v>895</v>
-      </c>
+        <v>897</v>
+      </c>
+      <c r="F47" s="20">
+        <v>2</v>
+      </c>
+      <c r="G47" s="20"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
       <c r="K47" s="20"/>
       <c r="L47" s="20"/>
       <c r="M47" s="20"/>
@@ -5973,10 +5963,10 @@
         <v>559</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>873</v>
+        <v>17</v>
       </c>
       <c r="G48" s="20" t="s">
-        <v>866</v>
+        <v>2</v>
       </c>
       <c r="H48" s="23"/>
       <c r="I48" s="20"/>
@@ -5986,7 +5976,7 @@
       <c r="M48" s="20"/>
       <c r="N48" s="16"/>
     </row>
-    <row r="49" spans="3:14" s="18" customFormat="1">
+    <row r="49" spans="3:14" s="18" customFormat="1" ht="14.25">
       <c r="C49" s="3">
         <v>48</v>
       </c>
@@ -5994,17 +5984,15 @@
         <v>864</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>559</v>
+        <v>865</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>874</v>
+        <v>100</v>
       </c>
       <c r="G49" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="H49" s="23" t="s">
-        <v>887</v>
-      </c>
+        <v>866</v>
+      </c>
+      <c r="H49" s="15"/>
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
       <c r="K49" s="20"/>
@@ -6017,13 +6005,13 @@
         <v>49</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>864</v>
+        <v>830</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>559</v>
+        <v>19</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G50" s="20" t="s">
         <v>2</v>
@@ -6041,28 +6029,26 @@
         <v>50</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>864</v>
+        <v>830</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>865</v>
+        <v>19</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>621</v>
+        <v>79</v>
       </c>
       <c r="G51" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H51" s="20" t="s">
-        <v>881</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H51" s="23"/>
       <c r="I51" s="20"/>
       <c r="J51" s="20"/>
       <c r="K51" s="20"/>
       <c r="L51" s="20"/>
       <c r="M51" s="20"/>
-      <c r="N51" s="27"/>
+      <c r="N51" s="16"/>
     </row>
-    <row r="52" spans="3:14" s="18" customFormat="1" ht="14.25">
+    <row r="52" spans="3:14" s="18" customFormat="1">
       <c r="C52" s="3">
         <v>51</v>
       </c>
@@ -6073,12 +6059,14 @@
         <v>865</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>203</v>
+        <v>621</v>
       </c>
       <c r="G52" s="20" t="s">
-        <v>866</v>
-      </c>
-      <c r="H52" s="15"/>
+        <v>56</v>
+      </c>
+      <c r="H52" s="20" t="s">
+        <v>881</v>
+      </c>
       <c r="I52" s="20"/>
       <c r="J52" s="20"/>
       <c r="K52" s="20"/>
@@ -6086,7 +6074,7 @@
       <c r="M52" s="20"/>
       <c r="N52" s="27"/>
     </row>
-    <row r="53" spans="3:14" s="18" customFormat="1">
+    <row r="53" spans="3:14" s="18" customFormat="1" ht="14.25">
       <c r="C53" s="3">
         <v>52</v>
       </c>
@@ -6094,21 +6082,21 @@
         <v>864</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>559</v>
+        <v>865</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>867</v>
+        <v>203</v>
       </c>
       <c r="G53" s="20" t="s">
         <v>866</v>
       </c>
-      <c r="H53" s="20"/>
+      <c r="H53" s="15"/>
       <c r="I53" s="20"/>
       <c r="J53" s="20"/>
       <c r="K53" s="20"/>
       <c r="L53" s="20"/>
       <c r="M53" s="20"/>
-      <c r="N53" s="16"/>
+      <c r="N53" s="27"/>
     </row>
     <row r="54" spans="3:14" s="18" customFormat="1">
       <c r="C54" s="3">
@@ -6121,20 +6109,14 @@
         <v>559</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="G54" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H54" s="23" t="s">
-        <v>854</v>
-      </c>
-      <c r="I54" s="23" t="s">
-        <v>851</v>
-      </c>
-      <c r="J54" s="20" t="b">
-        <v>1</v>
-      </c>
+        <v>866</v>
+      </c>
+      <c r="H54" s="20"/>
+      <c r="I54" s="20"/>
+      <c r="J54" s="20"/>
       <c r="K54" s="20"/>
       <c r="L54" s="20"/>
       <c r="M54" s="20"/>
@@ -6151,19 +6133,19 @@
         <v>559</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>874</v>
-      </c>
-      <c r="G55" s="23" t="s">
-        <v>885</v>
+        <v>870</v>
+      </c>
+      <c r="G55" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="H55" s="23" t="s">
-        <v>886</v>
+        <v>854</v>
       </c>
       <c r="I55" s="23" t="s">
         <v>851</v>
       </c>
-      <c r="J55" s="23" t="s">
-        <v>887</v>
+      <c r="J55" s="20" t="b">
+        <v>1</v>
       </c>
       <c r="K55" s="20"/>
       <c r="L55" s="20"/>
@@ -6181,14 +6163,20 @@
         <v>559</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>873</v>
-      </c>
-      <c r="G56" s="20" t="s">
-        <v>866</v>
-      </c>
-      <c r="H56" s="23"/>
-      <c r="I56" s="20"/>
-      <c r="J56" s="20"/>
+        <v>874</v>
+      </c>
+      <c r="G56" s="23" t="s">
+        <v>885</v>
+      </c>
+      <c r="H56" s="23" t="s">
+        <v>886</v>
+      </c>
+      <c r="I56" s="23" t="s">
+        <v>851</v>
+      </c>
+      <c r="J56" s="23" t="s">
+        <v>895</v>
+      </c>
       <c r="K56" s="20"/>
       <c r="L56" s="20"/>
       <c r="M56" s="20"/>
@@ -6205,14 +6193,12 @@
         <v>559</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="G57" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="H57" s="23" t="s">
-        <v>888</v>
-      </c>
+        <v>866</v>
+      </c>
+      <c r="H57" s="23"/>
       <c r="I57" s="20"/>
       <c r="J57" s="20"/>
       <c r="K57" s="20"/>
@@ -6231,12 +6217,14 @@
         <v>559</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>17</v>
+        <v>874</v>
       </c>
       <c r="G58" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H58" s="23"/>
+        <v>4</v>
+      </c>
+      <c r="H58" s="23" t="s">
+        <v>887</v>
+      </c>
       <c r="I58" s="20"/>
       <c r="J58" s="20"/>
       <c r="K58" s="20"/>
@@ -6244,7 +6232,7 @@
       <c r="M58" s="20"/>
       <c r="N58" s="16"/>
     </row>
-    <row r="59" spans="3:14" s="18" customFormat="1">
+    <row r="59" spans="3:14" s="18" customFormat="1" ht="14.25">
       <c r="C59" s="3">
         <v>58</v>
       </c>
@@ -6252,25 +6240,23 @@
         <v>864</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>865</v>
+        <v>559</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>621</v>
+        <v>874</v>
       </c>
       <c r="G59" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H59" s="20" t="s">
-        <v>860</v>
-      </c>
+        <v>866</v>
+      </c>
+      <c r="H59" s="15"/>
       <c r="I59" s="20"/>
       <c r="J59" s="20"/>
       <c r="K59" s="20"/>
       <c r="L59" s="20"/>
       <c r="M59" s="20"/>
-      <c r="N59" s="27"/>
+      <c r="N59" s="16"/>
     </row>
-    <row r="60" spans="3:14" s="18" customFormat="1" ht="14.25">
+    <row r="60" spans="3:14" s="18" customFormat="1">
       <c r="C60" s="3">
         <v>59</v>
       </c>
@@ -6278,23 +6264,23 @@
         <v>864</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>865</v>
+        <v>559</v>
       </c>
       <c r="F60" s="20" t="s">
-        <v>203</v>
+        <v>17</v>
       </c>
       <c r="G60" s="20" t="s">
-        <v>866</v>
-      </c>
-      <c r="H60" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="H60" s="23"/>
       <c r="I60" s="20"/>
       <c r="J60" s="20"/>
       <c r="K60" s="20"/>
       <c r="L60" s="20"/>
       <c r="M60" s="20"/>
-      <c r="N60" s="27"/>
+      <c r="N60" s="16"/>
     </row>
-    <row r="61" spans="3:14" s="18" customFormat="1">
+    <row r="61" spans="3:14" s="18" customFormat="1" ht="18.75" customHeight="1">
       <c r="C61" s="3">
         <v>60</v>
       </c>
@@ -6302,15 +6288,15 @@
         <v>864</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>559</v>
+        <v>865</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>867</v>
+        <v>100</v>
       </c>
       <c r="G61" s="20" t="s">
         <v>866</v>
       </c>
-      <c r="H61" s="20"/>
+      <c r="H61" s="15"/>
       <c r="I61" s="20"/>
       <c r="J61" s="20"/>
       <c r="K61" s="20"/>
@@ -6323,26 +6309,20 @@
         <v>61</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>864</v>
+        <v>830</v>
       </c>
       <c r="E62" s="23" t="s">
-        <v>559</v>
+        <v>19</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>870</v>
+        <v>22</v>
       </c>
       <c r="G62" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H62" s="23" t="s">
-        <v>854</v>
-      </c>
-      <c r="I62" s="23" t="s">
-        <v>851</v>
-      </c>
-      <c r="J62" s="20" t="b">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H62" s="23"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="20"/>
       <c r="K62" s="20"/>
       <c r="L62" s="20"/>
       <c r="M62" s="20"/>
@@ -6353,26 +6333,20 @@
         <v>62</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>864</v>
+        <v>830</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>559</v>
+        <v>19</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>874</v>
-      </c>
-      <c r="G63" s="23" t="s">
-        <v>885</v>
-      </c>
-      <c r="H63" s="23" t="s">
-        <v>886</v>
-      </c>
-      <c r="I63" s="23" t="s">
-        <v>851</v>
-      </c>
-      <c r="J63" s="23" t="s">
-        <v>883</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="G63" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H63" s="23"/>
+      <c r="I63" s="20"/>
+      <c r="J63" s="20"/>
       <c r="K63" s="20"/>
       <c r="L63" s="20"/>
       <c r="M63" s="20"/>
@@ -6386,74 +6360,66 @@
         <v>864</v>
       </c>
       <c r="E64" s="23" t="s">
-        <v>559</v>
+        <v>865</v>
       </c>
       <c r="F64" s="20" t="s">
-        <v>872</v>
+        <v>621</v>
       </c>
       <c r="G64" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H64" s="23" t="s">
-        <v>855</v>
-      </c>
-      <c r="I64" s="23" t="s">
-        <v>851</v>
-      </c>
-      <c r="J64" s="20" t="b">
-        <v>1</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H64" s="20" t="s">
+        <v>881</v>
+      </c>
+      <c r="I64" s="20"/>
+      <c r="J64" s="20"/>
       <c r="K64" s="20"/>
       <c r="L64" s="20"/>
       <c r="M64" s="20"/>
-      <c r="N64" s="16"/>
+      <c r="N64" s="27"/>
     </row>
-    <row r="65" spans="3:14" s="18" customFormat="1">
+    <row r="65" spans="3:14" s="18" customFormat="1" ht="14.25">
       <c r="C65" s="3">
         <v>64</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>896</v>
+        <v>864</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>559</v>
+        <v>865</v>
       </c>
       <c r="F65" s="20" t="s">
-        <v>872</v>
-      </c>
-      <c r="G65" s="23" t="s">
-        <v>884</v>
-      </c>
-      <c r="H65" s="23" t="s">
-        <v>887</v>
-      </c>
-      <c r="I65" s="23"/>
+        <v>203</v>
+      </c>
+      <c r="G65" s="20" t="s">
+        <v>866</v>
+      </c>
+      <c r="H65" s="15"/>
+      <c r="I65" s="20"/>
       <c r="J65" s="20"/>
       <c r="K65" s="20"/>
       <c r="L65" s="20"/>
       <c r="M65" s="20"/>
-      <c r="N65" s="16"/>
+      <c r="N65" s="27"/>
     </row>
     <row r="66" spans="3:14" s="18" customFormat="1">
       <c r="C66" s="3">
         <v>65</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>896</v>
+        <v>864</v>
       </c>
       <c r="E66" s="23" t="s">
         <v>559</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>872</v>
-      </c>
-      <c r="G66" s="23" t="s">
-        <v>884</v>
-      </c>
-      <c r="H66" s="23" t="s">
-        <v>888</v>
-      </c>
-      <c r="I66" s="23"/>
+        <v>867</v>
+      </c>
+      <c r="G66" s="20" t="s">
+        <v>866</v>
+      </c>
+      <c r="H66" s="20"/>
+      <c r="I66" s="20"/>
       <c r="J66" s="20"/>
       <c r="K66" s="20"/>
       <c r="L66" s="20"/>
@@ -6471,14 +6437,20 @@
         <v>559</v>
       </c>
       <c r="F67" s="20" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="G67" s="20" t="s">
-        <v>866</v>
-      </c>
-      <c r="H67" s="23"/>
-      <c r="I67" s="20"/>
-      <c r="J67" s="20"/>
+        <v>7</v>
+      </c>
+      <c r="H67" s="23" t="s">
+        <v>854</v>
+      </c>
+      <c r="I67" s="20" t="s">
+        <v>853</v>
+      </c>
+      <c r="J67" s="20" t="b">
+        <v>1</v>
+      </c>
       <c r="K67" s="20"/>
       <c r="L67" s="20"/>
       <c r="M67" s="20"/>
@@ -6497,14 +6469,18 @@
       <c r="F68" s="20" t="s">
         <v>874</v>
       </c>
-      <c r="G68" s="20" t="s">
-        <v>4</v>
+      <c r="G68" s="23" t="s">
+        <v>885</v>
       </c>
       <c r="H68" s="23" t="s">
-        <v>889</v>
-      </c>
-      <c r="I68" s="20"/>
-      <c r="J68" s="20"/>
+        <v>886</v>
+      </c>
+      <c r="I68" s="23" t="s">
+        <v>851</v>
+      </c>
+      <c r="J68" s="23" t="s">
+        <v>887</v>
+      </c>
       <c r="K68" s="20"/>
       <c r="L68" s="20"/>
       <c r="M68" s="20"/>
@@ -6521,10 +6497,10 @@
         <v>559</v>
       </c>
       <c r="F69" s="20" t="s">
-        <v>17</v>
+        <v>873</v>
       </c>
       <c r="G69" s="20" t="s">
-        <v>2</v>
+        <v>866</v>
       </c>
       <c r="H69" s="23"/>
       <c r="I69" s="20"/>
@@ -6542,23 +6518,23 @@
         <v>864</v>
       </c>
       <c r="E70" s="23" t="s">
-        <v>865</v>
+        <v>559</v>
       </c>
       <c r="F70" s="20" t="s">
-        <v>621</v>
+        <v>874</v>
       </c>
       <c r="G70" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H70" s="20" t="s">
-        <v>860</v>
+        <v>4</v>
+      </c>
+      <c r="H70" s="23" t="s">
+        <v>888</v>
       </c>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
       <c r="K70" s="20"/>
       <c r="L70" s="20"/>
       <c r="M70" s="20"/>
-      <c r="N70" s="27"/>
+      <c r="N70" s="16"/>
     </row>
     <row r="71" spans="3:14" s="18" customFormat="1" ht="14.25">
       <c r="C71" s="3">
@@ -6568,10 +6544,10 @@
         <v>864</v>
       </c>
       <c r="E71" s="23" t="s">
-        <v>865</v>
+        <v>559</v>
       </c>
       <c r="F71" s="20" t="s">
-        <v>213</v>
+        <v>874</v>
       </c>
       <c r="G71" s="20" t="s">
         <v>866</v>
@@ -6582,7 +6558,7 @@
       <c r="K71" s="20"/>
       <c r="L71" s="20"/>
       <c r="M71" s="20"/>
-      <c r="N71" s="27"/>
+      <c r="N71" s="16"/>
     </row>
     <row r="72" spans="3:14" s="18" customFormat="1">
       <c r="C72" s="3">
@@ -6592,15 +6568,15 @@
         <v>864</v>
       </c>
       <c r="E72" s="23" t="s">
-        <v>628</v>
+        <v>559</v>
       </c>
       <c r="F72" s="20" t="s">
-        <v>890</v>
+        <v>17</v>
       </c>
       <c r="G72" s="20" t="s">
-        <v>891</v>
-      </c>
-      <c r="H72" s="20"/>
+        <v>2</v>
+      </c>
+      <c r="H72" s="23"/>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
       <c r="K72" s="20"/>
@@ -6608,21 +6584,23 @@
       <c r="M72" s="20"/>
       <c r="N72" s="16"/>
     </row>
-    <row r="73" spans="3:14" s="18" customFormat="1">
+    <row r="73" spans="3:14" s="18" customFormat="1" ht="18.75" customHeight="1">
       <c r="C73" s="3">
         <v>72</v>
       </c>
       <c r="D73" s="22" t="s">
-        <v>892</v>
+        <v>864</v>
       </c>
       <c r="E73" s="23" t="s">
-        <v>799</v>
-      </c>
-      <c r="F73" s="20">
-        <v>2</v>
-      </c>
-      <c r="G73" s="20"/>
-      <c r="H73" s="23"/>
+        <v>865</v>
+      </c>
+      <c r="F73" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G73" s="20" t="s">
+        <v>866</v>
+      </c>
+      <c r="H73" s="15"/>
       <c r="I73" s="20"/>
       <c r="J73" s="20"/>
       <c r="K73" s="20"/>
@@ -6635,50 +6613,48 @@
         <v>73</v>
       </c>
       <c r="D74" s="22" t="s">
-        <v>864</v>
+        <v>830</v>
       </c>
       <c r="E74" s="23" t="s">
-        <v>865</v>
+        <v>19</v>
       </c>
       <c r="F74" s="20" t="s">
-        <v>621</v>
+        <v>22</v>
       </c>
       <c r="G74" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H74" s="20" t="s">
-        <v>881</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H74" s="23"/>
       <c r="I74" s="20"/>
       <c r="J74" s="20"/>
       <c r="K74" s="20"/>
       <c r="L74" s="20"/>
       <c r="M74" s="20"/>
-      <c r="N74" s="27"/>
+      <c r="N74" s="16"/>
     </row>
-    <row r="75" spans="3:14" s="18" customFormat="1" ht="14.25">
+    <row r="75" spans="3:14" s="18" customFormat="1">
       <c r="C75" s="3">
         <v>74</v>
       </c>
       <c r="D75" s="22" t="s">
-        <v>864</v>
+        <v>830</v>
       </c>
       <c r="E75" s="23" t="s">
-        <v>865</v>
+        <v>19</v>
       </c>
       <c r="F75" s="20" t="s">
-        <v>203</v>
+        <v>79</v>
       </c>
       <c r="G75" s="20" t="s">
-        <v>866</v>
-      </c>
-      <c r="H75" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="H75" s="23"/>
       <c r="I75" s="20"/>
       <c r="J75" s="20"/>
       <c r="K75" s="20"/>
       <c r="L75" s="20"/>
       <c r="M75" s="20"/>
-      <c r="N75" s="27"/>
+      <c r="N75" s="16"/>
     </row>
     <row r="76" spans="3:14" s="18" customFormat="1">
       <c r="C76" s="3">
@@ -6688,23 +6664,25 @@
         <v>864</v>
       </c>
       <c r="E76" s="23" t="s">
-        <v>559</v>
+        <v>865</v>
       </c>
       <c r="F76" s="20" t="s">
-        <v>867</v>
+        <v>621</v>
       </c>
       <c r="G76" s="20" t="s">
-        <v>866</v>
-      </c>
-      <c r="H76" s="20"/>
+        <v>56</v>
+      </c>
+      <c r="H76" s="20" t="s">
+        <v>860</v>
+      </c>
       <c r="I76" s="20"/>
       <c r="J76" s="20"/>
       <c r="K76" s="20"/>
       <c r="L76" s="20"/>
       <c r="M76" s="20"/>
-      <c r="N76" s="16"/>
+      <c r="N76" s="27"/>
     </row>
-    <row r="77" spans="3:14" s="18" customFormat="1">
+    <row r="77" spans="3:14" s="18" customFormat="1" ht="14.25">
       <c r="C77" s="3">
         <v>76</v>
       </c>
@@ -6712,27 +6690,21 @@
         <v>864</v>
       </c>
       <c r="E77" s="23" t="s">
-        <v>559</v>
+        <v>865</v>
       </c>
       <c r="F77" s="20" t="s">
-        <v>870</v>
+        <v>203</v>
       </c>
       <c r="G77" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H77" s="23" t="s">
-        <v>854</v>
-      </c>
-      <c r="I77" s="23" t="s">
-        <v>851</v>
-      </c>
-      <c r="J77" s="20" t="b">
-        <v>1</v>
-      </c>
+        <v>866</v>
+      </c>
+      <c r="H77" s="15"/>
+      <c r="I77" s="20"/>
+      <c r="J77" s="20"/>
       <c r="K77" s="20"/>
       <c r="L77" s="20"/>
       <c r="M77" s="20"/>
-      <c r="N77" s="16"/>
+      <c r="N77" s="27"/>
     </row>
     <row r="78" spans="3:14" s="18" customFormat="1">
       <c r="C78" s="3">
@@ -6745,20 +6717,14 @@
         <v>559</v>
       </c>
       <c r="F78" s="20" t="s">
-        <v>874</v>
-      </c>
-      <c r="G78" s="23" t="s">
-        <v>885</v>
-      </c>
-      <c r="H78" s="23" t="s">
-        <v>886</v>
-      </c>
-      <c r="I78" s="23" t="s">
-        <v>851</v>
-      </c>
-      <c r="J78" s="23" t="s">
-        <v>888</v>
-      </c>
+        <v>867</v>
+      </c>
+      <c r="G78" s="20" t="s">
+        <v>866</v>
+      </c>
+      <c r="H78" s="20"/>
+      <c r="I78" s="20"/>
+      <c r="J78" s="20"/>
       <c r="K78" s="20"/>
       <c r="L78" s="20"/>
       <c r="M78" s="20"/>
@@ -6775,14 +6741,20 @@
         <v>559</v>
       </c>
       <c r="F79" s="20" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="G79" s="20" t="s">
-        <v>866</v>
-      </c>
-      <c r="H79" s="23"/>
-      <c r="I79" s="20"/>
-      <c r="J79" s="20"/>
+        <v>7</v>
+      </c>
+      <c r="H79" s="23" t="s">
+        <v>854</v>
+      </c>
+      <c r="I79" s="20" t="s">
+        <v>853</v>
+      </c>
+      <c r="J79" s="20" t="b">
+        <v>1</v>
+      </c>
       <c r="K79" s="20"/>
       <c r="L79" s="20"/>
       <c r="M79" s="20"/>
@@ -6799,333 +6771,869 @@
         <v>559</v>
       </c>
       <c r="F80" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G80" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H80" s="23"/>
-      <c r="I80" s="20"/>
-      <c r="J80" s="20"/>
+        <v>874</v>
+      </c>
+      <c r="G80" s="23" t="s">
+        <v>885</v>
+      </c>
+      <c r="H80" s="23" t="s">
+        <v>886</v>
+      </c>
+      <c r="I80" s="23" t="s">
+        <v>851</v>
+      </c>
+      <c r="J80" s="23" t="s">
+        <v>883</v>
+      </c>
       <c r="K80" s="20"/>
       <c r="L80" s="20"/>
       <c r="M80" s="20"/>
       <c r="N80" s="16"/>
     </row>
-    <row r="81" spans="1:15" s="18" customFormat="1" ht="15">
+    <row r="81" spans="3:14" s="18" customFormat="1">
       <c r="C81" s="3">
         <v>80</v>
       </c>
-      <c r="D81" s="14" t="s">
-        <v>832</v>
-      </c>
-      <c r="E81" s="5"/>
-      <c r="F81" s="3"/>
-      <c r="G81" s="3"/>
-      <c r="H81" s="3"/>
-      <c r="I81" s="3"/>
-      <c r="J81" s="3"/>
-      <c r="K81" s="3"/>
-      <c r="L81" s="3"/>
-      <c r="M81" s="3"/>
+      <c r="D81" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="E81" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="F81" s="20" t="s">
+        <v>872</v>
+      </c>
+      <c r="G81" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H81" s="23" t="s">
+        <v>855</v>
+      </c>
+      <c r="I81" s="23" t="s">
+        <v>851</v>
+      </c>
+      <c r="J81" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K81" s="20"/>
+      <c r="L81" s="20"/>
+      <c r="M81" s="20"/>
       <c r="N81" s="16"/>
     </row>
-    <row r="82" spans="1:15" s="18" customFormat="1">
+    <row r="82" spans="3:14" s="18" customFormat="1">
       <c r="C82" s="3">
         <v>81</v>
       </c>
-      <c r="D82" s="12" t="s">
-        <v>847</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>848</v>
-      </c>
-      <c r="F82" s="3">
-        <v>5</v>
-      </c>
-      <c r="G82" s="3"/>
-      <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
-      <c r="J82" s="3"/>
-      <c r="K82" s="3"/>
-      <c r="L82" s="3"/>
-      <c r="M82" s="3"/>
+      <c r="D82" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="E82" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="F82" s="20" t="s">
+        <v>872</v>
+      </c>
+      <c r="G82" s="23" t="s">
+        <v>884</v>
+      </c>
+      <c r="H82" s="23" t="s">
+        <v>887</v>
+      </c>
+      <c r="I82" s="23"/>
+      <c r="J82" s="20"/>
+      <c r="K82" s="20"/>
+      <c r="L82" s="20"/>
+      <c r="M82" s="20"/>
       <c r="N82" s="16"/>
     </row>
-    <row r="83" spans="1:15" s="18" customFormat="1">
+    <row r="83" spans="3:14" s="18" customFormat="1">
       <c r="C83" s="3">
         <v>82</v>
       </c>
-      <c r="D83" s="12" t="s">
-        <v>830</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F83" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H83" s="5"/>
-      <c r="I83" s="5"/>
-      <c r="J83" s="3"/>
-      <c r="K83" s="3"/>
-      <c r="L83" s="3"/>
-      <c r="M83" s="3"/>
+      <c r="D83" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="E83" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="F83" s="20" t="s">
+        <v>872</v>
+      </c>
+      <c r="G83" s="23" t="s">
+        <v>884</v>
+      </c>
+      <c r="H83" s="23" t="s">
+        <v>888</v>
+      </c>
+      <c r="I83" s="23"/>
+      <c r="J83" s="20"/>
+      <c r="K83" s="20"/>
+      <c r="L83" s="20"/>
+      <c r="M83" s="20"/>
       <c r="N83" s="16"/>
     </row>
-    <row r="84" spans="1:15" s="18" customFormat="1">
+    <row r="84" spans="3:14" s="18" customFormat="1">
       <c r="C84" s="3">
         <v>83</v>
       </c>
-      <c r="D84" s="12" t="s">
-        <v>834</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H84" s="5"/>
-      <c r="I84" s="5"/>
-      <c r="J84" s="3"/>
-      <c r="K84" s="3"/>
-      <c r="L84" s="3"/>
-      <c r="M84" s="3"/>
+      <c r="D84" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="E84" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="F84" s="20" t="s">
+        <v>873</v>
+      </c>
+      <c r="G84" s="20" t="s">
+        <v>866</v>
+      </c>
+      <c r="H84" s="23"/>
+      <c r="I84" s="20"/>
+      <c r="J84" s="20"/>
+      <c r="K84" s="20"/>
+      <c r="L84" s="20"/>
+      <c r="M84" s="20"/>
       <c r="N84" s="16"/>
     </row>
-    <row r="85" spans="1:15" s="18" customFormat="1">
+    <row r="85" spans="3:14" s="18" customFormat="1">
       <c r="C85" s="3">
         <v>84</v>
       </c>
-      <c r="D85" s="12" t="s">
-        <v>834</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>835</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>621</v>
-      </c>
-      <c r="G85" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>833</v>
-      </c>
-      <c r="I85" s="3"/>
-      <c r="J85" s="3"/>
-      <c r="K85" s="3"/>
-      <c r="L85" s="3"/>
-      <c r="M85" s="3"/>
+      <c r="D85" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="E85" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="F85" s="20" t="s">
+        <v>874</v>
+      </c>
+      <c r="G85" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H85" s="23" t="s">
+        <v>889</v>
+      </c>
+      <c r="I85" s="20"/>
+      <c r="J85" s="20"/>
+      <c r="K85" s="20"/>
+      <c r="L85" s="20"/>
+      <c r="M85" s="20"/>
       <c r="N85" s="16"/>
     </row>
-    <row r="86" spans="1:15" s="18" customFormat="1" ht="14.25">
+    <row r="86" spans="3:14" s="18" customFormat="1" ht="14.25">
       <c r="C86" s="3">
         <v>85</v>
       </c>
-      <c r="D86" s="12" t="s">
-        <v>834</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>835</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H86" s="17"/>
-      <c r="I86" s="3"/>
-      <c r="J86" s="3"/>
-      <c r="K86" s="3"/>
-      <c r="L86" s="3"/>
-      <c r="M86" s="3"/>
+      <c r="D86" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="E86" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="F86" s="20" t="s">
+        <v>874</v>
+      </c>
+      <c r="G86" s="20" t="s">
+        <v>866</v>
+      </c>
+      <c r="H86" s="15"/>
+      <c r="I86" s="20"/>
+      <c r="J86" s="20"/>
+      <c r="K86" s="20"/>
+      <c r="L86" s="20"/>
+      <c r="M86" s="20"/>
       <c r="N86" s="16"/>
     </row>
-    <row r="87" spans="1:15" s="18" customFormat="1">
+    <row r="87" spans="3:14" s="18" customFormat="1">
       <c r="C87" s="3">
         <v>86</v>
       </c>
-      <c r="D87" s="12" t="s">
-        <v>834</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>628</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H87" s="5"/>
-      <c r="I87" s="3"/>
-      <c r="J87" s="3"/>
-      <c r="K87" s="3"/>
-      <c r="L87" s="3"/>
-      <c r="M87" s="3"/>
+      <c r="D87" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="E87" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="F87" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G87" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H87" s="23"/>
+      <c r="I87" s="20"/>
+      <c r="J87" s="20"/>
+      <c r="K87" s="20"/>
+      <c r="L87" s="20"/>
+      <c r="M87" s="20"/>
       <c r="N87" s="16"/>
     </row>
-    <row r="88" spans="1:15" s="18" customFormat="1">
+    <row r="88" spans="3:14" s="18" customFormat="1" ht="18.75" customHeight="1">
       <c r="C88" s="3">
         <v>87</v>
       </c>
-      <c r="D88" s="12" t="s">
-        <v>834</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>835</v>
-      </c>
-      <c r="F88" s="3" t="s">
+      <c r="D88" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="E88" s="23" t="s">
+        <v>865</v>
+      </c>
+      <c r="F88" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G88" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H88" s="5"/>
-      <c r="I88" s="5"/>
-      <c r="J88" s="3"/>
-      <c r="K88" s="3"/>
-      <c r="L88" s="3"/>
-      <c r="M88" s="3"/>
+      <c r="G88" s="20" t="s">
+        <v>866</v>
+      </c>
+      <c r="H88" s="15"/>
+      <c r="I88" s="20"/>
+      <c r="J88" s="20"/>
+      <c r="K88" s="20"/>
+      <c r="L88" s="20"/>
+      <c r="M88" s="20"/>
       <c r="N88" s="16"/>
     </row>
-    <row r="89" spans="1:15" s="18" customFormat="1">
+    <row r="89" spans="3:14" s="18" customFormat="1">
       <c r="C89" s="3">
         <v>88</v>
       </c>
-      <c r="D89" s="12" t="s">
+      <c r="D89" s="22" t="s">
         <v>830</v>
       </c>
-      <c r="E89" s="20" t="s">
+      <c r="E89" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F89" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G89" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H89" s="3"/>
-      <c r="I89" s="3"/>
-      <c r="J89" s="3"/>
-      <c r="K89" s="3"/>
-      <c r="L89" s="3"/>
-      <c r="M89" s="3"/>
+      <c r="G89" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H89" s="23"/>
+      <c r="I89" s="20"/>
+      <c r="J89" s="20"/>
+      <c r="K89" s="20"/>
+      <c r="L89" s="20"/>
+      <c r="M89" s="20"/>
       <c r="N89" s="16"/>
     </row>
-    <row r="90" spans="1:15" s="18" customFormat="1">
+    <row r="90" spans="3:14" s="18" customFormat="1">
       <c r="C90" s="3">
         <v>89</v>
       </c>
       <c r="D90" s="22" t="s">
         <v>830</v>
       </c>
-      <c r="E90" s="20" t="s">
+      <c r="E90" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F90" s="20" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G90" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H90" s="20"/>
+      <c r="H90" s="23"/>
       <c r="I90" s="20"/>
       <c r="J90" s="20"/>
       <c r="K90" s="20"/>
       <c r="L90" s="20"/>
       <c r="M90" s="20"/>
-      <c r="N90" s="21"/>
+      <c r="N90" s="16"/>
     </row>
-    <row r="91" spans="1:15" s="18" customFormat="1">
+    <row r="91" spans="3:14" s="18" customFormat="1">
       <c r="C91" s="3">
         <v>90</v>
       </c>
       <c r="D91" s="22" t="s">
-        <v>830</v>
-      </c>
-      <c r="E91" s="20" t="s">
-        <v>437</v>
+        <v>864</v>
+      </c>
+      <c r="E91" s="23" t="s">
+        <v>865</v>
       </c>
       <c r="F91" s="20" t="s">
-        <v>453</v>
+        <v>621</v>
       </c>
       <c r="G91" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="H91" s="23" t="s">
-        <v>893</v>
-      </c>
-      <c r="I91" s="23"/>
+        <v>56</v>
+      </c>
+      <c r="H91" s="20" t="s">
+        <v>860</v>
+      </c>
+      <c r="I91" s="20"/>
       <c r="J91" s="20"/>
       <c r="K91" s="20"/>
       <c r="L91" s="20"/>
       <c r="M91" s="20"/>
-      <c r="N91" s="21"/>
+      <c r="N91" s="27"/>
     </row>
-    <row r="92" spans="1:15" s="18" customFormat="1">
-      <c r="A92" s="13"/>
-      <c r="B92" s="13"/>
+    <row r="92" spans="3:14" s="18" customFormat="1" ht="14.25">
       <c r="C92" s="3">
         <v>91</v>
       </c>
       <c r="D92" s="22" t="s">
-        <v>830</v>
-      </c>
-      <c r="E92" s="20" t="s">
-        <v>437</v>
+        <v>864</v>
+      </c>
+      <c r="E92" s="23" t="s">
+        <v>865</v>
       </c>
       <c r="F92" s="20" t="s">
-        <v>452</v>
+        <v>213</v>
       </c>
       <c r="G92" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="H92" s="20"/>
+        <v>866</v>
+      </c>
+      <c r="H92" s="15"/>
       <c r="I92" s="20"/>
       <c r="J92" s="20"/>
       <c r="K92" s="20"/>
       <c r="L92" s="20"/>
       <c r="M92" s="20"/>
-      <c r="N92" s="21"/>
-      <c r="O92" s="19"/>
+      <c r="N92" s="27"/>
     </row>
-    <row r="93" spans="1:15" s="18" customFormat="1">
+    <row r="93" spans="3:14" s="18" customFormat="1">
       <c r="C93" s="3">
         <v>92</v>
       </c>
       <c r="D93" s="22" t="s">
-        <v>830</v>
-      </c>
-      <c r="E93" s="20" t="s">
-        <v>437</v>
+        <v>864</v>
+      </c>
+      <c r="E93" s="23" t="s">
+        <v>628</v>
       </c>
       <c r="F93" s="20" t="s">
-        <v>17</v>
+        <v>890</v>
       </c>
       <c r="G93" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H93" s="23"/>
+        <v>891</v>
+      </c>
+      <c r="H93" s="20"/>
       <c r="I93" s="20"/>
       <c r="J93" s="20"/>
       <c r="K93" s="20"/>
       <c r="L93" s="20"/>
       <c r="M93" s="20"/>
-      <c r="N93" s="21"/>
+      <c r="N93" s="16"/>
+    </row>
+    <row r="94" spans="3:14" s="18" customFormat="1">
+      <c r="C94" s="3">
+        <v>93</v>
+      </c>
+      <c r="D94" s="22" t="s">
+        <v>892</v>
+      </c>
+      <c r="E94" s="23" t="s">
+        <v>799</v>
+      </c>
+      <c r="F94" s="20">
+        <v>2</v>
+      </c>
+      <c r="G94" s="20"/>
+      <c r="H94" s="23"/>
+      <c r="I94" s="20"/>
+      <c r="J94" s="20"/>
+      <c r="K94" s="20"/>
+      <c r="L94" s="20"/>
+      <c r="M94" s="20"/>
+      <c r="N94" s="16"/>
+    </row>
+    <row r="95" spans="3:14" s="18" customFormat="1">
+      <c r="C95" s="3">
+        <v>94</v>
+      </c>
+      <c r="D95" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="E95" s="23" t="s">
+        <v>865</v>
+      </c>
+      <c r="F95" s="20" t="s">
+        <v>621</v>
+      </c>
+      <c r="G95" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="H95" s="20" t="s">
+        <v>881</v>
+      </c>
+      <c r="I95" s="20"/>
+      <c r="J95" s="20"/>
+      <c r="K95" s="20"/>
+      <c r="L95" s="20"/>
+      <c r="M95" s="20"/>
+      <c r="N95" s="27"/>
+    </row>
+    <row r="96" spans="3:14" s="18" customFormat="1" ht="14.25">
+      <c r="C96" s="3">
+        <v>95</v>
+      </c>
+      <c r="D96" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="E96" s="23" t="s">
+        <v>865</v>
+      </c>
+      <c r="F96" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="G96" s="20" t="s">
+        <v>866</v>
+      </c>
+      <c r="H96" s="15"/>
+      <c r="I96" s="20"/>
+      <c r="J96" s="20"/>
+      <c r="K96" s="20"/>
+      <c r="L96" s="20"/>
+      <c r="M96" s="20"/>
+      <c r="N96" s="27"/>
+    </row>
+    <row r="97" spans="3:14" s="18" customFormat="1">
+      <c r="C97" s="3">
+        <v>96</v>
+      </c>
+      <c r="D97" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="E97" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="F97" s="20" t="s">
+        <v>867</v>
+      </c>
+      <c r="G97" s="20" t="s">
+        <v>866</v>
+      </c>
+      <c r="H97" s="20"/>
+      <c r="I97" s="20"/>
+      <c r="J97" s="20"/>
+      <c r="K97" s="20"/>
+      <c r="L97" s="20"/>
+      <c r="M97" s="20"/>
+      <c r="N97" s="16"/>
+    </row>
+    <row r="98" spans="3:14" s="18" customFormat="1">
+      <c r="C98" s="3">
+        <v>97</v>
+      </c>
+      <c r="D98" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="E98" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="F98" s="20" t="s">
+        <v>870</v>
+      </c>
+      <c r="G98" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H98" s="23" t="s">
+        <v>854</v>
+      </c>
+      <c r="I98" s="20" t="s">
+        <v>853</v>
+      </c>
+      <c r="J98" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K98" s="20"/>
+      <c r="L98" s="20"/>
+      <c r="M98" s="20"/>
+      <c r="N98" s="16"/>
+    </row>
+    <row r="99" spans="3:14" s="18" customFormat="1">
+      <c r="C99" s="3">
+        <v>98</v>
+      </c>
+      <c r="D99" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="E99" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="F99" s="20" t="s">
+        <v>874</v>
+      </c>
+      <c r="G99" s="23" t="s">
+        <v>885</v>
+      </c>
+      <c r="H99" s="23" t="s">
+        <v>886</v>
+      </c>
+      <c r="I99" s="23" t="s">
+        <v>851</v>
+      </c>
+      <c r="J99" s="23" t="s">
+        <v>888</v>
+      </c>
+      <c r="K99" s="20"/>
+      <c r="L99" s="20"/>
+      <c r="M99" s="20"/>
+      <c r="N99" s="16"/>
+    </row>
+    <row r="100" spans="3:14" s="18" customFormat="1">
+      <c r="C100" s="3">
+        <v>99</v>
+      </c>
+      <c r="D100" s="22" t="s">
+        <v>898</v>
+      </c>
+      <c r="E100" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="F100" s="20" t="s">
+        <v>873</v>
+      </c>
+      <c r="G100" s="20" t="s">
+        <v>866</v>
+      </c>
+      <c r="H100" s="23"/>
+      <c r="I100" s="20"/>
+      <c r="J100" s="20"/>
+      <c r="K100" s="20"/>
+      <c r="L100" s="20"/>
+      <c r="M100" s="20"/>
+      <c r="N100" s="16"/>
+    </row>
+    <row r="101" spans="3:14" s="18" customFormat="1">
+      <c r="C101" s="3">
+        <v>100</v>
+      </c>
+      <c r="D101" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="E101" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="F101" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G101" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H101" s="23"/>
+      <c r="I101" s="20"/>
+      <c r="J101" s="20"/>
+      <c r="K101" s="20"/>
+      <c r="L101" s="20"/>
+      <c r="M101" s="20"/>
+      <c r="N101" s="16"/>
+    </row>
+    <row r="102" spans="3:14" s="18" customFormat="1" ht="15">
+      <c r="C102" s="3">
+        <v>101</v>
+      </c>
+      <c r="D102" s="14" t="s">
+        <v>832</v>
+      </c>
+      <c r="E102" s="5"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
+      <c r="I102" s="3"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="3"/>
+      <c r="M102" s="3"/>
+      <c r="N102" s="16"/>
+    </row>
+    <row r="103" spans="3:14" s="18" customFormat="1">
+      <c r="C103" s="3">
+        <v>102</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>847</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>848</v>
+      </c>
+      <c r="F103" s="3">
+        <v>5</v>
+      </c>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+      <c r="I103" s="3"/>
+      <c r="J103" s="3"/>
+      <c r="K103" s="3"/>
+      <c r="L103" s="3"/>
+      <c r="M103" s="3"/>
+      <c r="N103" s="16"/>
+    </row>
+    <row r="104" spans="3:14" s="18" customFormat="1">
+      <c r="C104" s="3">
+        <v>103</v>
+      </c>
+      <c r="D104" s="12" t="s">
+        <v>830</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H104" s="5"/>
+      <c r="I104" s="5"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="3"/>
+      <c r="M104" s="3"/>
+      <c r="N104" s="16"/>
+    </row>
+    <row r="105" spans="3:14" s="18" customFormat="1">
+      <c r="C105" s="3">
+        <v>104</v>
+      </c>
+      <c r="D105" s="12" t="s">
+        <v>834</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H105" s="5"/>
+      <c r="I105" s="5"/>
+      <c r="J105" s="3"/>
+      <c r="K105" s="3"/>
+      <c r="L105" s="3"/>
+      <c r="M105" s="3"/>
+      <c r="N105" s="16"/>
+    </row>
+    <row r="106" spans="3:14" s="18" customFormat="1">
+      <c r="C106" s="3">
+        <v>105</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>834</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>835</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H106" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="I106" s="3"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="3"/>
+      <c r="M106" s="3"/>
+      <c r="N106" s="16"/>
+    </row>
+    <row r="107" spans="3:14" s="18" customFormat="1" ht="14.25">
+      <c r="C107" s="3">
+        <v>106</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>834</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>835</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H107" s="17"/>
+      <c r="I107" s="3"/>
+      <c r="J107" s="3"/>
+      <c r="K107" s="3"/>
+      <c r="L107" s="3"/>
+      <c r="M107" s="3"/>
+      <c r="N107" s="16"/>
+    </row>
+    <row r="108" spans="3:14" s="18" customFormat="1">
+      <c r="C108" s="3">
+        <v>107</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>834</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H108" s="5"/>
+      <c r="I108" s="3"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="3"/>
+      <c r="M108" s="3"/>
+      <c r="N108" s="16"/>
+    </row>
+    <row r="109" spans="3:14" s="18" customFormat="1">
+      <c r="C109" s="3">
+        <v>108</v>
+      </c>
+      <c r="D109" s="12" t="s">
+        <v>834</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>835</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H109" s="5"/>
+      <c r="I109" s="5"/>
+      <c r="J109" s="3"/>
+      <c r="K109" s="3"/>
+      <c r="L109" s="3"/>
+      <c r="M109" s="3"/>
+      <c r="N109" s="16"/>
+    </row>
+    <row r="110" spans="3:14" s="18" customFormat="1">
+      <c r="C110" s="3">
+        <v>109</v>
+      </c>
+      <c r="D110" s="12" t="s">
+        <v>830</v>
+      </c>
+      <c r="E110" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F110" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H110" s="3"/>
+      <c r="I110" s="3"/>
+      <c r="J110" s="3"/>
+      <c r="K110" s="3"/>
+      <c r="L110" s="3"/>
+      <c r="M110" s="3"/>
+      <c r="N110" s="16"/>
+    </row>
+    <row r="111" spans="3:14" s="18" customFormat="1">
+      <c r="C111" s="3">
+        <v>110</v>
+      </c>
+      <c r="D111" s="22" t="s">
+        <v>830</v>
+      </c>
+      <c r="E111" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F111" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G111" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H111" s="20"/>
+      <c r="I111" s="20"/>
+      <c r="J111" s="20"/>
+      <c r="K111" s="20"/>
+      <c r="L111" s="20"/>
+      <c r="M111" s="20"/>
+      <c r="N111" s="21"/>
+    </row>
+    <row r="112" spans="3:14" s="18" customFormat="1">
+      <c r="C112" s="3">
+        <v>111</v>
+      </c>
+      <c r="D112" s="22" t="s">
+        <v>830</v>
+      </c>
+      <c r="E112" s="20" t="s">
+        <v>437</v>
+      </c>
+      <c r="F112" s="20" t="s">
+        <v>453</v>
+      </c>
+      <c r="G112" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H112" s="23" t="s">
+        <v>893</v>
+      </c>
+      <c r="I112" s="23"/>
+      <c r="J112" s="20"/>
+      <c r="K112" s="20"/>
+      <c r="L112" s="20"/>
+      <c r="M112" s="20"/>
+      <c r="N112" s="21"/>
+    </row>
+    <row r="113" spans="1:15" s="18" customFormat="1">
+      <c r="A113" s="13"/>
+      <c r="B113" s="13"/>
+      <c r="C113" s="3">
+        <v>112</v>
+      </c>
+      <c r="D113" s="22" t="s">
+        <v>830</v>
+      </c>
+      <c r="E113" s="20" t="s">
+        <v>437</v>
+      </c>
+      <c r="F113" s="20" t="s">
+        <v>452</v>
+      </c>
+      <c r="G113" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H113" s="20"/>
+      <c r="I113" s="20"/>
+      <c r="J113" s="20"/>
+      <c r="K113" s="20"/>
+      <c r="L113" s="20"/>
+      <c r="M113" s="20"/>
+      <c r="N113" s="21"/>
+      <c r="O113" s="19"/>
+    </row>
+    <row r="114" spans="1:15" s="18" customFormat="1">
+      <c r="C114" s="3">
+        <v>113</v>
+      </c>
+      <c r="D114" s="22" t="s">
+        <v>830</v>
+      </c>
+      <c r="E114" s="20" t="s">
+        <v>437</v>
+      </c>
+      <c r="F114" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G114" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H114" s="23"/>
+      <c r="I114" s="20"/>
+      <c r="J114" s="20"/>
+      <c r="K114" s="20"/>
+      <c r="L114" s="20"/>
+      <c r="M114" s="20"/>
+      <c r="N114" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="N2:N93">
+  <conditionalFormatting sqref="N2:N114">
     <cfRule type="cellIs" dxfId="1" priority="35" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
@@ -7134,16 +7642,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G28 G30:G37 G39:G40 G42:G46 G48:G54 G64 G56:G62 G67:G77 G79:G84 G86:G93">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G28 G47:G55 G107:G114 G57:G67 G44:G45 G81 G30:G42 G69:G79 G100:G105 G84:G98">
       <formula1>INDIRECT(SUBSTITUTE(E2&amp;F2," ",""))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F28:F35 F2:F25 F73:F75 F37:F44 F46:F52 F54:F60 F62:F71 F77:F93">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F98:F114 F2:F25 F94:F96 F55:F65 F67:F77 F42:F53 F28:F40 F79:F92">
       <formula1>OFFSET(INDIRECT($E2),0,0,COUNTA(INDIRECT(E2&amp;"Col")),1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D83 D10:D20 D22:D23 D3:D4 D89:D93">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D104 D10:D20 D22:D23 D3:D4 D110:D114 D37:D38 D50:D51 D62:D63 D74:D75 D89:D90">
       <formula1>"C,F,T,;"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E93">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E114">
       <formula1>Forms</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>